<commit_message>
Eclatement En marche bien
</commit_message>
<xml_diff>
--- a/public/uploads/Besoin.xlsx
+++ b/public/uploads/Besoin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\arco\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1316E8F-171A-4852-B4D8-0F8DC9A9D9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E87B60-76DA-4B86-9F9A-6BC442EC21AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="4200" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -29,435 +29,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="166">
-  <si>
-    <t>AS451</t>
-  </si>
-  <si>
-    <t>AS452</t>
-  </si>
-  <si>
-    <t>AS453</t>
-  </si>
-  <si>
-    <t>AS454</t>
-  </si>
-  <si>
-    <t>AS455</t>
-  </si>
-  <si>
-    <t>AS456</t>
-  </si>
-  <si>
-    <t>AS462</t>
-  </si>
-  <si>
-    <t>AS463</t>
-  </si>
-  <si>
-    <t>AS464</t>
-  </si>
-  <si>
-    <t>AS465</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>B120408</t>
-  </si>
-  <si>
-    <t>B120508</t>
-  </si>
-  <si>
-    <t>B120708</t>
-  </si>
-  <si>
-    <t>B120908</t>
-  </si>
-  <si>
-    <t>B121108</t>
-  </si>
-  <si>
-    <t>B121308</t>
-  </si>
-  <si>
-    <t>B121408</t>
-  </si>
-  <si>
-    <t>C30107</t>
-  </si>
-  <si>
-    <t>C30109</t>
-  </si>
-  <si>
-    <t>C30114</t>
-  </si>
-  <si>
-    <t>C30116</t>
-  </si>
-  <si>
-    <t>DE830C</t>
-  </si>
-  <si>
-    <t>KCM13</t>
-  </si>
-  <si>
-    <t>KCM14</t>
-  </si>
-  <si>
-    <t>KCM15</t>
-  </si>
-  <si>
-    <t>KCM16</t>
-  </si>
-  <si>
-    <t>KCM17</t>
-  </si>
-  <si>
-    <t>KCM18</t>
-  </si>
-  <si>
-    <t>KCM19</t>
-  </si>
-  <si>
-    <t>KCM45</t>
-  </si>
-  <si>
-    <t>KCM45SP</t>
-  </si>
-  <si>
-    <t>KCM48</t>
-  </si>
-  <si>
-    <t>MF210</t>
-  </si>
-  <si>
-    <t>NV870C</t>
-  </si>
-  <si>
-    <t>P2236</t>
-  </si>
-  <si>
-    <t>P2237</t>
-  </si>
-  <si>
-    <t>SA267</t>
-  </si>
-  <si>
-    <t>SEC4392</t>
-  </si>
-  <si>
-    <t>SE501215</t>
-  </si>
-  <si>
-    <t>SE501275</t>
-  </si>
-  <si>
-    <t>SE501285</t>
-  </si>
-  <si>
-    <t>SE501295</t>
-  </si>
-  <si>
-    <t>SE501615</t>
-  </si>
-  <si>
-    <t>SE503531</t>
-  </si>
-  <si>
-    <t>SE503555R</t>
-  </si>
-  <si>
-    <t>SE503556R</t>
-  </si>
-  <si>
-    <t>SE507205</t>
-  </si>
-  <si>
-    <t>SE507255</t>
-  </si>
-  <si>
-    <t>SE507531</t>
-  </si>
-  <si>
-    <t>SE507555R</t>
-  </si>
-  <si>
-    <t>SE507556R</t>
-  </si>
-  <si>
-    <t>SE507635</t>
-  </si>
-  <si>
-    <t>SL1111</t>
-  </si>
-  <si>
-    <t>SL1113</t>
-  </si>
-  <si>
-    <t>SL1116</t>
-  </si>
-  <si>
-    <t>SL1117</t>
-  </si>
-  <si>
-    <t>SL1132</t>
-  </si>
-  <si>
-    <t>SL1133</t>
-  </si>
-  <si>
-    <t>0046001</t>
-  </si>
-  <si>
-    <t>00462</t>
-  </si>
-  <si>
-    <t>00463</t>
-  </si>
-  <si>
-    <t>00472</t>
-  </si>
-  <si>
-    <t>0047201</t>
-  </si>
-  <si>
-    <t>0112308</t>
-  </si>
-  <si>
-    <t>0112408</t>
-  </si>
-  <si>
-    <t>0112608</t>
-  </si>
-  <si>
-    <t>0112708</t>
-  </si>
-  <si>
-    <t>0112808</t>
-  </si>
-  <si>
-    <t>0112908</t>
-  </si>
-  <si>
-    <t>0113108</t>
-  </si>
-  <si>
-    <t>0113108B</t>
-  </si>
-  <si>
-    <t>0113508</t>
-  </si>
-  <si>
-    <t>0113708</t>
-  </si>
-  <si>
-    <t>0113808</t>
-  </si>
-  <si>
-    <t>0120308</t>
-  </si>
-  <si>
-    <t>0120408</t>
-  </si>
-  <si>
-    <t>0120508</t>
-  </si>
-  <si>
-    <t>0120708</t>
-  </si>
-  <si>
-    <t>0120908</t>
-  </si>
-  <si>
-    <t>0121008</t>
-  </si>
-  <si>
-    <t>0121108</t>
-  </si>
-  <si>
-    <t>0121308</t>
-  </si>
-  <si>
-    <t>0121408</t>
-  </si>
-  <si>
-    <t>0121508</t>
-  </si>
-  <si>
-    <t>02229</t>
-  </si>
-  <si>
-    <t>02236</t>
-  </si>
-  <si>
-    <t>02267</t>
-  </si>
-  <si>
-    <t>02267U</t>
-  </si>
-  <si>
-    <t>02285</t>
-  </si>
-  <si>
-    <t>0233510</t>
-  </si>
-  <si>
-    <t>02400MAC</t>
-  </si>
-  <si>
-    <t>02400MAC02</t>
-  </si>
-  <si>
-    <t>02402MAC</t>
-  </si>
-  <si>
-    <t>02402MAC02</t>
-  </si>
-  <si>
-    <t>1TECH</t>
-  </si>
-  <si>
-    <t>1007711</t>
-  </si>
-  <si>
-    <t>1300186</t>
-  </si>
-  <si>
-    <t>1301280</t>
-  </si>
-  <si>
-    <t>1330320</t>
-  </si>
-  <si>
-    <t>1420151</t>
-  </si>
-  <si>
-    <t>1420280</t>
-  </si>
-  <si>
-    <t>191208</t>
-  </si>
-  <si>
-    <t>2TECH</t>
-  </si>
-  <si>
-    <t>201015</t>
-  </si>
-  <si>
-    <t>20101501</t>
-  </si>
-  <si>
-    <t>208020</t>
-  </si>
-  <si>
-    <t>212005U</t>
-  </si>
-  <si>
-    <t>36115</t>
-  </si>
-  <si>
-    <t>36320</t>
-  </si>
-  <si>
-    <t>36330</t>
-  </si>
-  <si>
-    <t>36420</t>
-  </si>
-  <si>
-    <t>37515</t>
-  </si>
-  <si>
-    <t>37525</t>
-  </si>
-  <si>
-    <t>37720</t>
-  </si>
-  <si>
-    <t>5TECH</t>
-  </si>
-  <si>
-    <t>501215</t>
-  </si>
-  <si>
-    <t>501275</t>
-  </si>
-  <si>
-    <t>501285</t>
-  </si>
-  <si>
-    <t>503200</t>
-  </si>
-  <si>
-    <t>503205</t>
-  </si>
-  <si>
-    <t>503210</t>
-  </si>
-  <si>
-    <t>503215</t>
-  </si>
-  <si>
-    <t>503255</t>
-  </si>
-  <si>
-    <t>503265</t>
-  </si>
-  <si>
-    <t>503270</t>
-  </si>
-  <si>
-    <t>503505</t>
-  </si>
-  <si>
-    <t>507205</t>
-  </si>
-  <si>
-    <t>507210</t>
-  </si>
-  <si>
-    <t>507215</t>
-  </si>
-  <si>
-    <t>507255</t>
-  </si>
-  <si>
-    <t>507265</t>
-  </si>
-  <si>
-    <t>507305</t>
-  </si>
-  <si>
-    <t>507340</t>
-  </si>
-  <si>
-    <t>507365</t>
-  </si>
-  <si>
-    <t>507505</t>
-  </si>
-  <si>
-    <t>876010</t>
-  </si>
-  <si>
-    <t>876020</t>
-  </si>
-  <si>
-    <t>876040</t>
-  </si>
-  <si>
-    <t>876220</t>
-  </si>
-  <si>
-    <t>876240</t>
-  </si>
-  <si>
-    <t>876410</t>
-  </si>
-  <si>
-    <t>876420</t>
-  </si>
-  <si>
-    <t>876440</t>
   </si>
   <si>
     <t>id</t>
@@ -527,6 +101,108 @@
   </si>
   <si>
     <t>s1</t>
+  </si>
+  <si>
+    <t>1007710</t>
+  </si>
+  <si>
+    <t>1301300M</t>
+  </si>
+  <si>
+    <t>1301300E</t>
+  </si>
+  <si>
+    <t>1000702E</t>
+  </si>
+  <si>
+    <t>1030004</t>
+  </si>
+  <si>
+    <t>1007708</t>
+  </si>
+  <si>
+    <t>1030357</t>
+  </si>
+  <si>
+    <t>1030185</t>
+  </si>
+  <si>
+    <t>1030358</t>
+  </si>
+  <si>
+    <t>1007596</t>
+  </si>
+  <si>
+    <t>1031139</t>
+  </si>
+  <si>
+    <t>1007622</t>
+  </si>
+  <si>
+    <t>1033129</t>
+  </si>
+  <si>
+    <t>1007620</t>
+  </si>
+  <si>
+    <t>1033131</t>
+  </si>
+  <si>
+    <t>1007628</t>
+  </si>
+  <si>
+    <t>1033133</t>
+  </si>
+  <si>
+    <t>1009950E</t>
+  </si>
+  <si>
+    <t>1009910E</t>
+  </si>
+  <si>
+    <t>1009940G</t>
+  </si>
+  <si>
+    <t>1300178</t>
+  </si>
+  <si>
+    <t>1009941M</t>
+  </si>
+  <si>
+    <t>1009920M</t>
+  </si>
+  <si>
+    <t>1300069MP</t>
+  </si>
+  <si>
+    <t>1309548M</t>
+  </si>
+  <si>
+    <t>1300179E</t>
+  </si>
+  <si>
+    <t>1008900E</t>
+  </si>
+  <si>
+    <t>1309548E</t>
+  </si>
+  <si>
+    <t>1000701E</t>
+  </si>
+  <si>
+    <t>1030007</t>
+  </si>
+  <si>
+    <t>1007624</t>
+  </si>
+  <si>
+    <t>1030166</t>
+  </si>
+  <si>
+    <t>1030187</t>
+  </si>
+  <si>
+    <t>1008880E</t>
   </si>
 </sst>
 </file>
@@ -908,7 +584,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1021,6 +697,15 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1150,7 +835,7 @@
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1161,7 +846,9 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="124">
     <cellStyle name="20 % - Accent1" xfId="100" builtinId="30" customBuiltin="1"/>
@@ -1568,86 +1255,86 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:W349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>150</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>155</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="Q1" t="s">
-        <v>159</v>
+        <v>17</v>
       </c>
       <c r="R1" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="S1" t="s">
-        <v>161</v>
+        <v>19</v>
       </c>
       <c r="T1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="U1" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="V1" t="s">
-        <v>164</v>
+        <v>22</v>
       </c>
       <c r="W1" t="s">
-        <v>156</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5">
@@ -8471,92 +8158,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17ACAE54-B3E6-44BA-9EA0-30D1932E1BEF}">
   <dimension ref="A1:W349"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="7"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>143</v>
-      </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>150</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>151</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>155</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="P1" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="Q1" t="s">
-        <v>159</v>
+        <v>17</v>
       </c>
       <c r="R1" t="s">
-        <v>160</v>
+        <v>18</v>
       </c>
       <c r="S1" t="s">
-        <v>161</v>
+        <v>19</v>
       </c>
       <c r="T1" t="s">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="U1" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="V1" t="s">
-        <v>164</v>
+        <v>22</v>
       </c>
       <c r="W1" t="s">
-        <v>156</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="7" t="s">
+        <v>27</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6">
+        <v>433</v>
+      </c>
       <c r="C2" s="6">
-        <v>1448</v>
+        <v>433</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <v>433</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -8573,14 +8264,12 @@
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
+      <c r="A3" s="8" t="s">
+        <v>28</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5">
-        <v>1323</v>
+      <c r="D3" s="3">
+        <v>0</v>
       </c>
-      <c r="D3" s="3"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -8597,14 +8286,18 @@
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
+      <c r="A4" s="8" t="s">
+        <v>29</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5">
-        <v>5817</v>
+      <c r="B4" s="6">
+        <v>7211</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="C4" s="6">
+        <v>7211</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7211</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -8621,14 +8314,14 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+      <c r="A5" s="8" t="s">
+        <v>30</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5">
-        <v>10080</v>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3">
+        <v>0</v>
       </c>
-      <c r="D5" s="3"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -8645,14 +8338,14 @@
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
+      <c r="A6" s="8" t="s">
+        <v>24</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5">
-        <v>20622</v>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3">
+        <v>0</v>
       </c>
-      <c r="D6" s="3"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -8669,14 +8362,14 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+      <c r="A7" s="8" t="s">
+        <v>31</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5">
-        <v>9429</v>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3">
+        <v>0</v>
       </c>
-      <c r="D7" s="3"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -8693,14 +8386,12 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
+      <c r="A8" s="8" t="s">
+        <v>32</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5">
-        <v>84</v>
+      <c r="D8" s="3">
+        <v>0</v>
       </c>
-      <c r="D8" s="3"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -8717,14 +8408,18 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
+      <c r="A9" s="8" t="s">
+        <v>33</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5">
-        <v>21</v>
+      <c r="B9">
+        <v>687</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="C9">
+        <v>687</v>
+      </c>
+      <c r="D9" s="3">
+        <v>687</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -8741,14 +8436,18 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
+      <c r="A10" s="8" t="s">
+        <v>34</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5">
-        <v>2310</v>
+      <c r="B10">
+        <v>3106</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="C10">
+        <v>3106</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3106</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -8765,14 +8464,18 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+      <c r="A11" s="8" t="s">
+        <v>35</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5">
-        <v>132</v>
+      <c r="B11" s="6">
+        <v>1474</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="C11" s="6">
+        <v>1474</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1474</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -8789,14 +8492,18 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
+      <c r="A12" s="8" t="s">
+        <v>36</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5">
-        <v>240</v>
+      <c r="B12">
+        <v>1221</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="C12">
+        <v>1221</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1221</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -8813,14 +8520,18 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
+      <c r="A13" s="8" t="s">
+        <v>37</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5">
-        <v>2500</v>
+      <c r="B13">
+        <v>1152</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="C13">
+        <v>1152</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1152</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -8837,14 +8548,12 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
+      <c r="A14" s="8" t="s">
+        <v>38</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5">
-        <v>1400</v>
+      <c r="D14" s="3">
+        <v>0</v>
       </c>
-      <c r="D14" s="3"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -8861,14 +8570,12 @@
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
+      <c r="A15" s="8" t="s">
+        <v>39</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5">
-        <v>900</v>
+      <c r="D15" s="3">
+        <v>0</v>
       </c>
-      <c r="D15" s="3"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -8885,14 +8592,12 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
+      <c r="A16" s="8" t="s">
+        <v>40</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5">
-        <v>312</v>
+      <c r="D16" s="3">
+        <v>0</v>
       </c>
-      <c r="D16" s="3"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -8909,14 +8614,18 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
+      <c r="A17" s="8" t="s">
+        <v>26</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5">
-        <v>320</v>
+      <c r="B17">
+        <v>24150</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="C17">
+        <v>24150</v>
+      </c>
+      <c r="D17" s="3">
+        <v>24150</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -8933,14 +8642,18 @@
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
+      <c r="A18" s="8" t="s">
+        <v>41</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5">
-        <v>160</v>
+      <c r="B18">
+        <v>300</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="C18">
+        <v>300</v>
+      </c>
+      <c r="D18" s="3">
+        <v>300</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -8957,14 +8670,18 @@
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
+      <c r="A19" s="8" t="s">
+        <v>42</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5">
-        <v>192</v>
+      <c r="B19">
+        <v>3050</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="C19">
+        <v>3050</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3050</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -8981,14 +8698,12 @@
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
+      <c r="A20" s="8" t="s">
+        <v>43</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5">
-        <v>480</v>
+      <c r="D20" s="3">
+        <v>0</v>
       </c>
-      <c r="D20" s="3"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -9005,14 +8720,14 @@
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
+      <c r="A21" s="8" t="s">
+        <v>44</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5">
-        <v>1170</v>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3">
+        <v>0</v>
       </c>
-      <c r="D21" s="3"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -9029,14 +8744,18 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
+      <c r="A22" s="8" t="s">
+        <v>25</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5">
-        <v>192</v>
+      <c r="B22">
+        <v>581</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="C22">
+        <v>581</v>
+      </c>
+      <c r="D22" s="3">
+        <v>581</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -9053,14 +8772,14 @@
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>21</v>
+      <c r="A23" s="8" t="s">
+        <v>45</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5">
-        <v>5600</v>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="3">
+        <v>0</v>
       </c>
-      <c r="D23" s="3"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -9077,14 +8796,14 @@
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>22</v>
+      <c r="A24" s="8" t="s">
+        <v>46</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5">
-        <v>90</v>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3">
+        <v>0</v>
       </c>
-      <c r="D24" s="3"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -9101,14 +8820,14 @@
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
+      <c r="A25" s="8" t="s">
+        <v>47</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5">
-        <v>300</v>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3">
+        <v>0</v>
       </c>
-      <c r="D25" s="3"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -9125,14 +8844,12 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
+      <c r="A26" s="8" t="s">
+        <v>48</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5">
-        <v>6630</v>
+      <c r="D26" s="3">
+        <v>0</v>
       </c>
-      <c r="D26" s="3"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -9149,14 +8866,18 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>25</v>
+      <c r="A27" s="8" t="s">
+        <v>49</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5">
-        <v>23850</v>
+      <c r="B27">
+        <v>823</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="C27">
+        <v>823</v>
+      </c>
+      <c r="D27" s="3">
+        <v>823</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -9173,14 +8894,12 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>26</v>
+      <c r="A28" s="8" t="s">
+        <v>50</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5">
-        <v>11130</v>
+      <c r="D28" s="3">
+        <v>0</v>
       </c>
-      <c r="D28" s="3"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -9197,14 +8916,14 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>27</v>
+      <c r="A29" s="8" t="s">
+        <v>51</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5">
-        <v>450</v>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="3">
+        <v>0</v>
       </c>
-      <c r="D29" s="3"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -9221,14 +8940,14 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>28</v>
+      <c r="A30" s="8" t="s">
+        <v>52</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5">
-        <v>300</v>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="3">
+        <v>0</v>
       </c>
-      <c r="D30" s="3"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -9245,14 +8964,18 @@
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>29</v>
+      <c r="A31" s="8" t="s">
+        <v>53</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5">
-        <v>1500</v>
+      <c r="B31">
+        <v>240</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="C31">
+        <v>240</v>
+      </c>
+      <c r="D31" s="3">
+        <v>240</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -9269,14 +8992,18 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
+      <c r="A32" s="8" t="s">
+        <v>54</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5">
-        <v>360</v>
+      <c r="B32">
+        <v>600</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="C32">
+        <v>600</v>
+      </c>
+      <c r="D32" s="3">
+        <v>600</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -9293,14 +9020,14 @@
       <c r="R32" s="1"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
+      <c r="A33" s="8" t="s">
+        <v>55</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5">
-        <v>330</v>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="3">
+        <v>0</v>
       </c>
-      <c r="D33" s="3"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -9317,14 +9044,14 @@
       <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
+      <c r="A34" s="8" t="s">
+        <v>56</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5">
-        <v>7400</v>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="3">
+        <v>0</v>
       </c>
-      <c r="D34" s="3"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -9341,14 +9068,12 @@
       <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
+      <c r="A35" s="8" t="s">
+        <v>57</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5">
-        <v>12857</v>
+      <c r="D35" s="3">
+        <v>0</v>
       </c>
-      <c r="D35" s="3"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -9365,13 +9090,7 @@
       <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5">
-        <v>2100</v>
-      </c>
+      <c r="A36" s="8"/>
       <c r="D36" s="3"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -9389,13 +9108,7 @@
       <c r="R36" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5">
-        <v>500</v>
-      </c>
+      <c r="A37" s="8"/>
       <c r="D37" s="3"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -9413,13 +9126,7 @@
       <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5">
-        <v>13500</v>
-      </c>
+      <c r="A38" s="8"/>
       <c r="D38" s="3"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -9437,13 +9144,9 @@
       <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5">
-        <v>2550</v>
-      </c>
+      <c r="A39" s="8"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="3"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -9461,13 +9164,9 @@
       <c r="R39" s="1"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5">
-        <v>4080</v>
-      </c>
+      <c r="A40" s="8"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="3"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -9485,13 +9184,7 @@
       <c r="R40" s="1"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5">
-        <v>1620</v>
-      </c>
+      <c r="A41" s="8"/>
       <c r="D41" s="3"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -9509,13 +9202,7 @@
       <c r="R41" s="1"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5">
-        <v>1320</v>
-      </c>
+      <c r="A42" s="8"/>
       <c r="D42" s="3"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -9533,13 +9220,7 @@
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5">
-        <v>120</v>
-      </c>
+      <c r="A43" s="8"/>
       <c r="D43" s="3"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -9557,13 +9238,7 @@
       <c r="R43" s="1"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5">
-        <v>900</v>
-      </c>
+      <c r="A44" s="8"/>
       <c r="D44" s="3"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -9581,13 +9256,7 @@
       <c r="R44" s="1"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5">
-        <v>540</v>
-      </c>
+      <c r="A45" s="8"/>
       <c r="D45" s="3"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -9605,13 +9274,7 @@
       <c r="R45" s="1"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5">
-        <v>840</v>
-      </c>
+      <c r="A46" s="8"/>
       <c r="D46" s="3"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -9629,13 +9292,7 @@
       <c r="R46" s="1"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5">
-        <v>230</v>
-      </c>
+      <c r="A47" s="8"/>
       <c r="D47" s="3"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -9653,13 +9310,7 @@
       <c r="R47" s="1"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5">
-        <v>4440</v>
-      </c>
+      <c r="A48" s="8"/>
       <c r="D48" s="3"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -9677,13 +9328,7 @@
       <c r="R48" s="1"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5">
-        <v>5970</v>
-      </c>
+      <c r="A49" s="8"/>
       <c r="D49" s="3"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -9701,13 +9346,7 @@
       <c r="R49" s="1"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5">
-        <v>506</v>
-      </c>
+      <c r="A50" s="8"/>
       <c r="D50" s="3"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -9725,13 +9364,7 @@
       <c r="R50" s="1"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5">
-        <v>960</v>
-      </c>
+      <c r="A51" s="8"/>
       <c r="D51" s="3"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -9749,13 +9382,9 @@
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5">
-        <v>304</v>
-      </c>
+      <c r="A52" s="8"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
       <c r="D52" s="3"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -9773,13 +9402,7 @@
       <c r="R52" s="1"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5">
-        <v>640</v>
-      </c>
+      <c r="A53" s="8"/>
       <c r="D53" s="3"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -9797,13 +9420,7 @@
       <c r="R53" s="1"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5">
-        <v>40</v>
-      </c>
+      <c r="A54" s="8"/>
       <c r="D54" s="3"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -9821,13 +9438,9 @@
       <c r="R54" s="1"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5">
-        <v>720</v>
-      </c>
+      <c r="A55" s="8"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
       <c r="D55" s="3"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -9845,13 +9458,9 @@
       <c r="R55" s="1"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5">
-        <v>72</v>
-      </c>
+      <c r="A56" s="8"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
       <c r="D56" s="3"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -9869,13 +9478,9 @@
       <c r="R56" s="1"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5">
-        <v>40</v>
-      </c>
+      <c r="A57" s="8"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
       <c r="D57" s="3"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -9893,13 +9498,9 @@
       <c r="R57" s="1"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5">
-        <v>450</v>
-      </c>
+      <c r="A58" s="8"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
       <c r="D58" s="3"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -9917,13 +9518,7 @@
       <c r="R58" s="1"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5">
-        <v>640</v>
-      </c>
+      <c r="A59" s="8"/>
       <c r="D59" s="3"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -9941,13 +9536,7 @@
       <c r="R59" s="1"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5">
-        <v>528</v>
-      </c>
+      <c r="A60" s="8"/>
       <c r="D60" s="3"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -9965,13 +9554,7 @@
       <c r="R60" s="1"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5">
-        <v>3600</v>
-      </c>
+      <c r="A61" s="8"/>
       <c r="D61" s="3"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -9989,13 +9572,9 @@
       <c r="R61" s="1"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5">
-        <v>360</v>
-      </c>
+      <c r="A62" s="8"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
       <c r="D62" s="3"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -10013,13 +9592,9 @@
       <c r="R62" s="1"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5">
-        <v>12960</v>
-      </c>
+      <c r="A63" s="8"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
       <c r="D63" s="3"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -10037,13 +9612,9 @@
       <c r="R63" s="1"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5">
-        <v>1080</v>
-      </c>
+      <c r="A64" s="8"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
       <c r="D64" s="3"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -10061,13 +9632,9 @@
       <c r="R64" s="1"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5">
-        <v>180</v>
-      </c>
+      <c r="A65" s="8"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
       <c r="D65" s="3"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -10085,13 +9652,7 @@
       <c r="R65" s="1"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5">
-        <v>480</v>
-      </c>
+      <c r="A66" s="8"/>
       <c r="D66" s="3"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -10109,13 +9670,9 @@
       <c r="R66" s="1"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5">
-        <v>600</v>
-      </c>
+      <c r="A67" s="8"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
       <c r="D67" s="3"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -10133,13 +9690,9 @@
       <c r="R67" s="1"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5">
-        <v>4500</v>
-      </c>
+      <c r="A68" s="8"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
       <c r="D68" s="3"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -10157,13 +9710,9 @@
       <c r="R68" s="1"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5">
-        <v>6750</v>
-      </c>
+      <c r="A69" s="8"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
       <c r="D69" s="3"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -10181,13 +9730,7 @@
       <c r="R69" s="1"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5">
-        <v>4200</v>
-      </c>
+      <c r="A70" s="8"/>
       <c r="D70" s="3"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -10205,13 +9748,7 @@
       <c r="R70" s="1"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5">
-        <v>300</v>
-      </c>
+      <c r="A71" s="8"/>
       <c r="D71" s="3"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -10229,13 +9766,7 @@
       <c r="R71" s="1"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5">
-        <v>5469</v>
-      </c>
+      <c r="A72" s="8"/>
       <c r="D72" s="3"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -10253,13 +9784,9 @@
       <c r="R72" s="1"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5">
-        <v>16</v>
-      </c>
+      <c r="A73" s="8"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
       <c r="D73" s="3"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -10277,13 +9804,9 @@
       <c r="R73" s="1"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5">
-        <v>400</v>
-      </c>
+      <c r="A74" s="8"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
       <c r="D74" s="3"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -10301,13 +9824,9 @@
       <c r="R74" s="1"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5">
-        <v>1600</v>
-      </c>
+      <c r="A75" s="8"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
       <c r="D75" s="3"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -10325,13 +9844,9 @@
       <c r="R75" s="1"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5">
-        <v>1200</v>
-      </c>
+      <c r="A76" s="8"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
       <c r="D76" s="3"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -10349,13 +9864,9 @@
       <c r="R76" s="1"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5">
-        <v>1860</v>
-      </c>
+      <c r="A77" s="8"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
       <c r="D77" s="3"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -10373,13 +9884,9 @@
       <c r="R77" s="1"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5">
-        <v>18000</v>
-      </c>
+      <c r="A78" s="8"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
       <c r="D78" s="3"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -10397,13 +9904,9 @@
       <c r="R78" s="1"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5">
-        <v>13480</v>
-      </c>
+      <c r="A79" s="8"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
       <c r="D79" s="3"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -10421,13 +9924,7 @@
       <c r="R79" s="1"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5">
-        <v>9660</v>
-      </c>
+      <c r="A80" s="8"/>
       <c r="D80" s="3"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -10445,13 +9942,7 @@
       <c r="R80" s="1"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81" s="5"/>
-      <c r="C81" s="5">
-        <v>1240</v>
-      </c>
+      <c r="A81" s="8"/>
       <c r="D81" s="3"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -10469,13 +9960,9 @@
       <c r="R81" s="1"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5">
-        <v>3780</v>
-      </c>
+      <c r="A82" s="8"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
       <c r="D82" s="3"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -10493,13 +9980,9 @@
       <c r="R82" s="1"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" s="5"/>
-      <c r="C83" s="5">
-        <v>2880</v>
-      </c>
+      <c r="A83" s="8"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
       <c r="D83" s="3"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -10517,13 +10000,9 @@
       <c r="R83" s="1"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B84" s="5"/>
-      <c r="C84" s="5">
-        <v>3060</v>
-      </c>
+      <c r="A84" s="8"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
       <c r="D84" s="3"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -10541,13 +10020,9 @@
       <c r="R84" s="1"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="5"/>
-      <c r="C85" s="5">
-        <v>160</v>
-      </c>
+      <c r="A85" s="8"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
       <c r="D85" s="3"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -10565,13 +10040,9 @@
       <c r="R85" s="1"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B86" s="5"/>
-      <c r="C86" s="5">
-        <v>500</v>
-      </c>
+      <c r="A86" s="8"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
       <c r="D86" s="3"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -10589,13 +10060,9 @@
       <c r="R86" s="1"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" s="5"/>
-      <c r="C87" s="5">
-        <v>1300</v>
-      </c>
+      <c r="A87" s="8"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
       <c r="D87" s="3"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -10613,13 +10080,9 @@
       <c r="R87" s="1"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B88" s="5"/>
-      <c r="C88" s="5">
-        <v>33000</v>
-      </c>
+      <c r="A88" s="8"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
       <c r="D88" s="3"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -10637,13 +10100,9 @@
       <c r="R88" s="1"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5">
-        <v>4100</v>
-      </c>
+      <c r="A89" s="8"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="6"/>
       <c r="D89" s="3"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -10661,13 +10120,9 @@
       <c r="R89" s="1"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5">
-        <v>2500</v>
-      </c>
+      <c r="A90" s="8"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
       <c r="D90" s="3"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -10685,13 +10140,9 @@
       <c r="R90" s="1"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5">
-        <v>15750</v>
-      </c>
+      <c r="A91" s="8"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="6"/>
       <c r="D91" s="3"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -10709,13 +10160,9 @@
       <c r="R91" s="1"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5">
-        <v>3960</v>
-      </c>
+      <c r="A92" s="8"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="6"/>
       <c r="D92" s="3"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -10733,13 +10180,9 @@
       <c r="R92" s="1"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5">
-        <v>1980</v>
-      </c>
+      <c r="A93" s="8"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
       <c r="D93" s="3"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -10757,13 +10200,9 @@
       <c r="R93" s="1"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B94" s="5"/>
-      <c r="C94" s="5">
-        <v>51980</v>
-      </c>
+      <c r="A94" s="8"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
       <c r="D94" s="3"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
@@ -10781,13 +10220,9 @@
       <c r="R94" s="1"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="5"/>
-      <c r="C95" s="5">
-        <v>7200</v>
-      </c>
+      <c r="A95" s="8"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
       <c r="D95" s="3"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
@@ -10805,13 +10240,7 @@
       <c r="R95" s="1"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5">
-        <v>200</v>
-      </c>
+      <c r="A96" s="8"/>
       <c r="D96" s="3"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -10829,13 +10258,9 @@
       <c r="R96" s="1"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5">
-        <v>0</v>
-      </c>
+      <c r="A97" s="8"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
       <c r="D97" s="3"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -10853,13 +10278,9 @@
       <c r="R97" s="1"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5">
-        <v>0</v>
-      </c>
+      <c r="A98" s="8"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
       <c r="D98" s="3"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -10877,13 +10298,9 @@
       <c r="R98" s="1"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B99" s="5"/>
-      <c r="C99" s="5">
-        <v>16731</v>
-      </c>
+      <c r="A99" s="8"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
       <c r="D99" s="3"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -10901,13 +10318,9 @@
       <c r="R99" s="1"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5">
-        <v>27457</v>
-      </c>
+      <c r="A100" s="8"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
       <c r="D100" s="3"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -10925,13 +10338,7 @@
       <c r="R100" s="1"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5">
-        <v>5000</v>
-      </c>
+      <c r="A101" s="8"/>
       <c r="D101" s="3"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -10949,13 +10356,9 @@
       <c r="R101" s="1"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5">
-        <v>29211</v>
-      </c>
+      <c r="A102" s="8"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
       <c r="D102" s="3"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -10973,13 +10376,9 @@
       <c r="R102" s="1"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B103" s="5"/>
-      <c r="C103" s="5">
-        <v>237</v>
-      </c>
+      <c r="A103" s="8"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
       <c r="D103" s="3"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -10997,13 +10396,9 @@
       <c r="R103" s="1"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B104" s="5"/>
-      <c r="C104" s="5">
-        <v>126</v>
-      </c>
+      <c r="A104" s="8"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
       <c r="D104" s="3"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -11021,13 +10416,7 @@
       <c r="R104" s="1"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5">
-        <v>1000</v>
-      </c>
+      <c r="A105" s="8"/>
       <c r="D105" s="3"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
@@ -11045,13 +10434,7 @@
       <c r="R105" s="1"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5">
-        <v>1000</v>
-      </c>
+      <c r="A106" s="8"/>
       <c r="D106" s="3"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -11069,13 +10452,7 @@
       <c r="R106" s="1"/>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B107" s="5"/>
-      <c r="C107" s="5">
-        <v>3000</v>
-      </c>
+      <c r="A107" s="8"/>
       <c r="D107" s="3"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -11093,13 +10470,7 @@
       <c r="R107" s="1"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B108" s="5"/>
-      <c r="C108" s="5">
-        <v>8700</v>
-      </c>
+      <c r="A108" s="8"/>
       <c r="D108" s="3"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -11117,13 +10488,7 @@
       <c r="R108" s="1"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B109" s="5"/>
-      <c r="C109" s="5">
-        <v>320</v>
-      </c>
+      <c r="A109" s="8"/>
       <c r="D109" s="3"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -11141,13 +10506,7 @@
       <c r="R109" s="1"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5">
-        <v>1200</v>
-      </c>
+      <c r="A110" s="8"/>
       <c r="D110" s="3"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -11165,13 +10524,9 @@
       <c r="R110" s="1"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B111" s="5"/>
-      <c r="C111" s="5">
-        <v>80</v>
-      </c>
+      <c r="A111" s="8"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
       <c r="D111" s="3"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -11189,13 +10544,7 @@
       <c r="R111" s="1"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B112" s="5"/>
-      <c r="C112" s="5">
-        <v>1580</v>
-      </c>
+      <c r="A112" s="8"/>
       <c r="D112" s="3"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -11213,13 +10562,7 @@
       <c r="R112" s="1"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5">
-        <v>363</v>
-      </c>
+      <c r="A113" s="8"/>
       <c r="D113" s="3"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -11237,13 +10580,7 @@
       <c r="R113" s="1"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5">
-        <v>41</v>
-      </c>
+      <c r="A114" s="8"/>
       <c r="D114" s="3"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -11261,13 +10598,9 @@
       <c r="R114" s="1"/>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5">
-        <v>600</v>
-      </c>
+      <c r="A115" s="8"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
       <c r="D115" s="3"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -11285,13 +10618,9 @@
       <c r="R115" s="1"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="A116" s="8"/>
       <c r="B116" s="5"/>
-      <c r="C116" s="5">
-        <v>4750</v>
-      </c>
+      <c r="C116" s="5"/>
       <c r="D116" s="3"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -11309,13 +10638,9 @@
       <c r="R116" s="1"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="A117" s="2"/>
       <c r="B117" s="5"/>
-      <c r="C117" s="5">
-        <v>360</v>
-      </c>
+      <c r="C117" s="5"/>
       <c r="D117" s="3"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -11333,13 +10658,9 @@
       <c r="R117" s="1"/>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="A118" s="2"/>
       <c r="B118" s="5"/>
-      <c r="C118" s="5">
-        <v>1200</v>
-      </c>
+      <c r="C118" s="5"/>
       <c r="D118" s="3"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -11357,13 +10678,9 @@
       <c r="R118" s="1"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>117</v>
-      </c>
+      <c r="A119" s="2"/>
       <c r="B119" s="5"/>
-      <c r="C119" s="5">
-        <v>60</v>
-      </c>
+      <c r="C119" s="5"/>
       <c r="D119" s="3"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -11381,13 +10698,9 @@
       <c r="R119" s="1"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>118</v>
-      </c>
+      <c r="A120" s="2"/>
       <c r="B120" s="5"/>
-      <c r="C120" s="5">
-        <v>1980</v>
-      </c>
+      <c r="C120" s="5"/>
       <c r="D120" s="3"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -11405,13 +10718,9 @@
       <c r="R120" s="1"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>119</v>
-      </c>
+      <c r="A121" s="2"/>
       <c r="B121" s="5"/>
-      <c r="C121" s="5">
-        <v>14340</v>
-      </c>
+      <c r="C121" s="5"/>
       <c r="D121" s="3"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -11429,13 +10738,9 @@
       <c r="R121" s="1"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>120</v>
-      </c>
+      <c r="A122" s="2"/>
       <c r="B122" s="5"/>
-      <c r="C122" s="5">
-        <v>48</v>
-      </c>
+      <c r="C122" s="5"/>
       <c r="D122" s="3"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -11453,13 +10758,9 @@
       <c r="R122" s="1"/>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>121</v>
-      </c>
+      <c r="A123" s="2"/>
       <c r="B123" s="5"/>
-      <c r="C123" s="5">
-        <v>1877</v>
-      </c>
+      <c r="C123" s="5"/>
       <c r="D123" s="3"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -11477,13 +10778,9 @@
       <c r="R123" s="1"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>122</v>
-      </c>
+      <c r="A124" s="2"/>
       <c r="B124" s="5"/>
-      <c r="C124" s="5">
-        <v>2460</v>
-      </c>
+      <c r="C124" s="5"/>
       <c r="D124" s="3"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -11501,13 +10798,9 @@
       <c r="R124" s="1"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="A125" s="2"/>
       <c r="B125" s="5"/>
-      <c r="C125" s="5">
-        <v>6420</v>
-      </c>
+      <c r="C125" s="5"/>
       <c r="D125" s="3"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -11525,13 +10818,9 @@
       <c r="R125" s="1"/>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="A126" s="2"/>
       <c r="B126" s="5"/>
-      <c r="C126" s="5">
-        <v>768</v>
-      </c>
+      <c r="C126" s="5"/>
       <c r="D126" s="3"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -11549,13 +10838,9 @@
       <c r="R126" s="1"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
-        <v>125</v>
-      </c>
+      <c r="A127" s="2"/>
       <c r="B127" s="5"/>
-      <c r="C127" s="5">
-        <v>540</v>
-      </c>
+      <c r="C127" s="5"/>
       <c r="D127" s="3"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -11573,13 +10858,9 @@
       <c r="R127" s="1"/>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>126</v>
-      </c>
+      <c r="A128" s="2"/>
       <c r="B128" s="5"/>
-      <c r="C128" s="5">
-        <v>12600</v>
-      </c>
+      <c r="C128" s="5"/>
       <c r="D128" s="3"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -11597,13 +10878,9 @@
       <c r="R128" s="1"/>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="A129" s="2"/>
       <c r="B129" s="5"/>
-      <c r="C129" s="5">
-        <v>192</v>
-      </c>
+      <c r="C129" s="5"/>
       <c r="D129" s="3"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -11621,13 +10898,9 @@
       <c r="R129" s="1"/>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>128</v>
-      </c>
+      <c r="A130" s="2"/>
       <c r="B130" s="5"/>
-      <c r="C130" s="5">
-        <v>900</v>
-      </c>
+      <c r="C130" s="5"/>
       <c r="D130" s="3"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -11645,13 +10918,9 @@
       <c r="R130" s="1"/>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="A131" s="2"/>
       <c r="B131" s="5"/>
-      <c r="C131" s="5">
-        <v>1680</v>
-      </c>
+      <c r="C131" s="5"/>
       <c r="D131" s="3"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -11669,13 +10938,9 @@
       <c r="R131" s="1"/>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="A132" s="2"/>
       <c r="B132" s="5"/>
-      <c r="C132" s="5">
-        <v>900</v>
-      </c>
+      <c r="C132" s="5"/>
       <c r="D132" s="3"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -11693,13 +10958,9 @@
       <c r="R132" s="1"/>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="A133" s="2"/>
       <c r="B133" s="5"/>
-      <c r="C133" s="5">
-        <v>5400</v>
-      </c>
+      <c r="C133" s="5"/>
       <c r="D133" s="3"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -11717,13 +10978,9 @@
       <c r="R133" s="1"/>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="A134" s="2"/>
       <c r="B134" s="5"/>
-      <c r="C134" s="5">
-        <v>20</v>
-      </c>
+      <c r="C134" s="5"/>
       <c r="D134" s="3"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -11741,13 +10998,9 @@
       <c r="R134" s="1"/>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="A135" s="2"/>
       <c r="B135" s="5"/>
-      <c r="C135" s="5">
-        <v>3600</v>
-      </c>
+      <c r="C135" s="5"/>
       <c r="D135" s="3"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -11765,13 +11018,9 @@
       <c r="R135" s="1"/>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="A136" s="2"/>
       <c r="B136" s="5"/>
-      <c r="C136" s="5">
-        <v>660</v>
-      </c>
+      <c r="C136" s="5"/>
       <c r="D136" s="3"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -11789,13 +11038,9 @@
       <c r="R136" s="1"/>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>135</v>
-      </c>
+      <c r="A137" s="2"/>
       <c r="B137" s="5"/>
-      <c r="C137" s="5">
-        <v>3607</v>
-      </c>
+      <c r="C137" s="5"/>
       <c r="D137" s="3"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -11813,13 +11058,9 @@
       <c r="R137" s="1"/>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>136</v>
-      </c>
+      <c r="A138" s="2"/>
       <c r="B138" s="5"/>
-      <c r="C138" s="5">
-        <v>6940</v>
-      </c>
+      <c r="C138" s="5"/>
       <c r="D138" s="3"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -11837,13 +11078,9 @@
       <c r="R138" s="1"/>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>137</v>
-      </c>
+      <c r="A139" s="2"/>
       <c r="B139" s="5"/>
-      <c r="C139" s="5">
-        <v>1520</v>
-      </c>
+      <c r="C139" s="5"/>
       <c r="D139" s="3"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -11861,13 +11098,9 @@
       <c r="R139" s="1"/>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>138</v>
-      </c>
+      <c r="A140" s="2"/>
       <c r="B140" s="5"/>
-      <c r="C140" s="5">
-        <v>2320</v>
-      </c>
+      <c r="C140" s="5"/>
       <c r="D140" s="3"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -11885,13 +11118,9 @@
       <c r="R140" s="1"/>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="A141" s="2"/>
       <c r="B141" s="5"/>
-      <c r="C141" s="5">
-        <v>140</v>
-      </c>
+      <c r="C141" s="5"/>
       <c r="D141" s="3"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -11909,13 +11138,9 @@
       <c r="R141" s="1"/>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>140</v>
-      </c>
+      <c r="A142" s="2"/>
       <c r="B142" s="5"/>
-      <c r="C142" s="5">
-        <v>4520</v>
-      </c>
+      <c r="C142" s="5"/>
       <c r="D142" s="3"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
@@ -11933,13 +11158,9 @@
       <c r="R142" s="1"/>
     </row>
     <row r="143" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>141</v>
-      </c>
+      <c r="A143" s="2"/>
       <c r="B143" s="5"/>
-      <c r="C143" s="5">
-        <v>4480</v>
-      </c>
+      <c r="C143" s="5"/>
       <c r="D143" s="3"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
@@ -11957,13 +11178,9 @@
       <c r="R143" s="1"/>
     </row>
     <row r="144" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="A144" s="2"/>
       <c r="B144" s="5"/>
-      <c r="C144" s="5">
-        <v>1840</v>
-      </c>
+      <c r="C144" s="5"/>
       <c r="D144" s="3"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -11982,7 +11199,6 @@
     </row>
     <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
-      <c r="C145" s="5"/>
       <c r="D145" s="3"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -12001,7 +11217,6 @@
     </row>
     <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
-      <c r="C146" s="5"/>
       <c r="D146" s="3"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
@@ -12020,7 +11235,6 @@
     </row>
     <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
-      <c r="C147" s="5"/>
       <c r="D147" s="3"/>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
@@ -12039,7 +11253,6 @@
     </row>
     <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
-      <c r="C148" s="5"/>
       <c r="D148" s="3"/>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
@@ -12058,7 +11271,6 @@
     </row>
     <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
-      <c r="C149" s="5"/>
       <c r="D149" s="3"/>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
@@ -12077,7 +11289,6 @@
     </row>
     <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
-      <c r="C150" s="5"/>
       <c r="D150" s="3"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
@@ -12096,7 +11307,6 @@
     </row>
     <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
-      <c r="C151" s="5"/>
       <c r="D151" s="3"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
@@ -12115,7 +11325,6 @@
     </row>
     <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
-      <c r="C152" s="5"/>
       <c r="D152" s="3"/>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
@@ -12134,7 +11343,6 @@
     </row>
     <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
-      <c r="C153" s="5"/>
       <c r="D153" s="3"/>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
@@ -12153,7 +11361,6 @@
     </row>
     <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
-      <c r="C154" s="5"/>
       <c r="D154" s="3"/>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
@@ -12172,7 +11379,6 @@
     </row>
     <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
-      <c r="C155" s="5"/>
       <c r="D155" s="3"/>
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
@@ -12191,7 +11397,6 @@
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
-      <c r="C156" s="5"/>
       <c r="D156" s="3"/>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
@@ -12210,7 +11415,6 @@
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
-      <c r="C157" s="5"/>
       <c r="D157" s="3"/>
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
@@ -12229,7 +11433,6 @@
     </row>
     <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
-      <c r="C158" s="5"/>
       <c r="D158" s="3"/>
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
@@ -12248,7 +11451,6 @@
     </row>
     <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
-      <c r="C159" s="5"/>
       <c r="D159" s="3"/>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
@@ -12267,7 +11469,6 @@
     </row>
     <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
-      <c r="C160" s="5"/>
       <c r="D160" s="3"/>
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
@@ -12286,7 +11487,6 @@
     </row>
     <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
-      <c r="C161" s="5"/>
       <c r="D161" s="3"/>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
@@ -12305,7 +11505,6 @@
     </row>
     <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
-      <c r="C162" s="5"/>
       <c r="D162" s="3"/>
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
@@ -12324,7 +11523,6 @@
     </row>
     <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
-      <c r="C163" s="5"/>
       <c r="D163" s="3"/>
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
@@ -12343,7 +11541,6 @@
     </row>
     <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
-      <c r="C164" s="5"/>
       <c r="D164" s="3"/>
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
@@ -12362,7 +11559,6 @@
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
-      <c r="C165" s="5"/>
       <c r="D165" s="3"/>
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
@@ -12381,7 +11577,6 @@
     </row>
     <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
-      <c r="C166" s="5"/>
       <c r="D166" s="3"/>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
@@ -12400,7 +11595,6 @@
     </row>
     <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
-      <c r="C167" s="5"/>
       <c r="D167" s="3"/>
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
@@ -12419,7 +11613,6 @@
     </row>
     <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
-      <c r="C168" s="5"/>
       <c r="D168" s="3"/>
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
@@ -12438,7 +11631,6 @@
     </row>
     <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
-      <c r="C169" s="5"/>
       <c r="D169" s="3"/>
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
@@ -12457,7 +11649,6 @@
     </row>
     <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
-      <c r="C170" s="5"/>
       <c r="D170" s="3"/>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
@@ -12476,7 +11667,6 @@
     </row>
     <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
-      <c r="C171" s="5"/>
       <c r="D171" s="3"/>
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
@@ -12495,7 +11685,6 @@
     </row>
     <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
-      <c r="C172" s="5"/>
       <c r="D172" s="3"/>
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
@@ -12514,7 +11703,6 @@
     </row>
     <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
-      <c r="C173" s="5"/>
       <c r="D173" s="3"/>
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
@@ -12533,7 +11721,6 @@
     </row>
     <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
-      <c r="C174" s="5"/>
       <c r="D174" s="3"/>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
@@ -12552,7 +11739,6 @@
     </row>
     <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
-      <c r="C175" s="5"/>
       <c r="D175" s="3"/>
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
@@ -12571,7 +11757,6 @@
     </row>
     <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
-      <c r="C176" s="5"/>
       <c r="D176" s="3"/>
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
@@ -12590,7 +11775,6 @@
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
-      <c r="C177" s="5"/>
       <c r="D177" s="3"/>
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
@@ -12609,7 +11793,6 @@
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
-      <c r="C178" s="5"/>
       <c r="D178" s="3"/>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
@@ -12628,7 +11811,6 @@
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
-      <c r="C179" s="5"/>
       <c r="D179" s="3"/>
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
@@ -12647,7 +11829,6 @@
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
-      <c r="C180" s="5"/>
       <c r="D180" s="3"/>
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
@@ -12666,7 +11847,6 @@
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
-      <c r="C181" s="5"/>
       <c r="D181" s="3"/>
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
@@ -12685,7 +11865,6 @@
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
-      <c r="C182" s="5"/>
       <c r="D182" s="3"/>
       <c r="E182" s="1"/>
       <c r="F182" s="1"/>
@@ -12704,7 +11883,6 @@
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
-      <c r="C183" s="5"/>
       <c r="D183" s="3"/>
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
@@ -12723,7 +11901,6 @@
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
-      <c r="C184" s="5"/>
       <c r="D184" s="3"/>
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
@@ -12742,7 +11919,6 @@
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
-      <c r="C185" s="5"/>
       <c r="D185" s="3"/>
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
@@ -12761,7 +11937,6 @@
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
-      <c r="C186" s="5"/>
       <c r="D186" s="3"/>
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
@@ -12780,7 +11955,6 @@
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
-      <c r="C187" s="5"/>
       <c r="D187" s="3"/>
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
@@ -12799,7 +11973,6 @@
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
-      <c r="C188" s="5"/>
       <c r="D188" s="3"/>
       <c r="E188" s="1"/>
       <c r="F188" s="1"/>
@@ -12818,7 +11991,6 @@
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
-      <c r="C189" s="5"/>
       <c r="D189" s="3"/>
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
@@ -12837,7 +12009,6 @@
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
-      <c r="C190" s="5"/>
       <c r="D190" s="3"/>
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
@@ -12856,7 +12027,6 @@
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
-      <c r="C191" s="5"/>
       <c r="D191" s="3"/>
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
@@ -12875,7 +12045,6 @@
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
-      <c r="C192" s="5"/>
       <c r="D192" s="3"/>
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
@@ -12894,7 +12063,6 @@
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
-      <c r="C193" s="5"/>
       <c r="D193" s="3"/>
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
@@ -12913,7 +12081,6 @@
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
-      <c r="C194" s="5"/>
       <c r="D194" s="3"/>
       <c r="E194" s="1"/>
       <c r="F194" s="1"/>
@@ -12932,7 +12099,6 @@
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
-      <c r="C195" s="5"/>
       <c r="D195" s="3"/>
       <c r="E195" s="1"/>
       <c r="F195" s="1"/>
@@ -12951,7 +12117,6 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
-      <c r="C196" s="5"/>
       <c r="D196" s="3"/>
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
@@ -12970,7 +12135,6 @@
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
-      <c r="C197" s="5"/>
       <c r="D197" s="3"/>
       <c r="E197" s="1"/>
       <c r="F197" s="1"/>
@@ -12989,7 +12153,6 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
-      <c r="C198" s="5"/>
       <c r="D198" s="3"/>
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
@@ -13008,7 +12171,6 @@
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
-      <c r="C199" s="5"/>
       <c r="D199" s="3"/>
       <c r="E199" s="1"/>
       <c r="F199" s="1"/>
@@ -13027,7 +12189,6 @@
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
-      <c r="C200" s="5"/>
       <c r="D200" s="3"/>
       <c r="E200" s="1"/>
       <c r="F200" s="1"/>
@@ -13046,7 +12207,6 @@
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
-      <c r="C201" s="5"/>
       <c r="D201" s="3"/>
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
@@ -13065,7 +12225,6 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
-      <c r="C202" s="5"/>
       <c r="D202" s="3"/>
       <c r="E202" s="1"/>
       <c r="F202" s="1"/>
@@ -13084,7 +12243,6 @@
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
-      <c r="C203" s="5"/>
       <c r="D203" s="3"/>
       <c r="E203" s="1"/>
       <c r="F203" s="1"/>
@@ -13103,7 +12261,6 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
-      <c r="C204" s="5"/>
       <c r="D204" s="3"/>
       <c r="E204" s="1"/>
       <c r="F204" s="1"/>
@@ -13122,7 +12279,6 @@
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
-      <c r="C205" s="5"/>
       <c r="D205" s="3"/>
       <c r="E205" s="1"/>
       <c r="F205" s="1"/>
@@ -13141,7 +12297,6 @@
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
-      <c r="C206" s="5"/>
       <c r="D206" s="3"/>
       <c r="E206" s="1"/>
       <c r="F206" s="1"/>
@@ -13160,7 +12315,6 @@
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
-      <c r="C207" s="5"/>
       <c r="D207" s="3"/>
       <c r="E207" s="1"/>
       <c r="F207" s="1"/>
@@ -13179,7 +12333,6 @@
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
-      <c r="C208" s="5"/>
       <c r="D208" s="3"/>
       <c r="E208" s="1"/>
       <c r="F208" s="1"/>
@@ -13198,7 +12351,6 @@
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
-      <c r="C209" s="5"/>
       <c r="D209" s="3"/>
       <c r="E209" s="1"/>
       <c r="F209" s="1"/>
@@ -13217,7 +12369,6 @@
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
-      <c r="C210" s="5"/>
       <c r="D210" s="3"/>
       <c r="E210" s="1"/>
       <c r="F210" s="1"/>
@@ -13236,7 +12387,6 @@
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
-      <c r="C211" s="5"/>
       <c r="D211" s="3"/>
       <c r="E211" s="1"/>
       <c r="F211" s="1"/>
@@ -13255,7 +12405,6 @@
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
-      <c r="C212" s="5"/>
       <c r="D212" s="3"/>
       <c r="E212" s="1"/>
       <c r="F212" s="1"/>
@@ -13274,7 +12423,6 @@
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
-      <c r="C213" s="5"/>
       <c r="D213" s="3"/>
       <c r="E213" s="1"/>
       <c r="F213" s="1"/>
@@ -13293,7 +12441,6 @@
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
-      <c r="C214" s="5"/>
       <c r="D214" s="3"/>
       <c r="E214" s="1"/>
       <c r="F214" s="1"/>
@@ -13312,7 +12459,6 @@
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
-      <c r="C215" s="5"/>
       <c r="D215" s="3"/>
       <c r="E215" s="1"/>
       <c r="F215" s="1"/>
@@ -13331,7 +12477,6 @@
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
-      <c r="C216" s="5"/>
       <c r="D216" s="3"/>
       <c r="E216" s="1"/>
       <c r="F216" s="1"/>
@@ -13350,7 +12495,6 @@
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
-      <c r="C217" s="5"/>
       <c r="D217" s="3"/>
       <c r="E217" s="1"/>
       <c r="F217" s="1"/>
@@ -13369,7 +12513,6 @@
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
-      <c r="C218" s="5"/>
       <c r="D218" s="3"/>
       <c r="E218" s="1"/>
       <c r="F218" s="1"/>
@@ -13388,7 +12531,6 @@
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
-      <c r="C219" s="5"/>
       <c r="D219" s="3"/>
       <c r="E219" s="1"/>
       <c r="F219" s="1"/>
@@ -13407,7 +12549,6 @@
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
-      <c r="C220" s="5"/>
       <c r="D220" s="3"/>
       <c r="E220" s="1"/>
       <c r="F220" s="1"/>
@@ -13426,7 +12567,6 @@
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
-      <c r="C221" s="5"/>
       <c r="D221" s="3"/>
       <c r="E221" s="1"/>
       <c r="F221" s="1"/>
@@ -13445,7 +12585,6 @@
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
-      <c r="C222" s="5"/>
       <c r="D222" s="3"/>
       <c r="E222" s="1"/>
       <c r="F222" s="1"/>
@@ -13464,7 +12603,6 @@
     </row>
     <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
-      <c r="C223" s="5"/>
       <c r="D223" s="3"/>
       <c r="E223" s="1"/>
       <c r="F223" s="1"/>
@@ -13483,7 +12621,6 @@
     </row>
     <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
-      <c r="C224" s="5"/>
       <c r="D224" s="3"/>
       <c r="E224" s="1"/>
       <c r="F224" s="1"/>
@@ -13502,7 +12639,6 @@
     </row>
     <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
-      <c r="C225" s="5"/>
       <c r="D225" s="3"/>
       <c r="E225" s="1"/>
       <c r="F225" s="1"/>
@@ -13521,7 +12657,6 @@
     </row>
     <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
-      <c r="C226" s="5"/>
       <c r="D226" s="3"/>
       <c r="E226" s="1"/>
       <c r="F226" s="1"/>
@@ -13540,7 +12675,6 @@
     </row>
     <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
-      <c r="C227" s="5"/>
       <c r="D227" s="3"/>
       <c r="E227" s="1"/>
       <c r="F227" s="1"/>
@@ -13559,7 +12693,6 @@
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
-      <c r="C228" s="5"/>
       <c r="D228" s="3"/>
       <c r="E228" s="1"/>
       <c r="F228" s="1"/>
@@ -13578,7 +12711,6 @@
     </row>
     <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
-      <c r="C229" s="5"/>
       <c r="D229" s="3"/>
       <c r="E229" s="1"/>
       <c r="F229" s="1"/>
@@ -13597,7 +12729,6 @@
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
-      <c r="C230" s="5"/>
       <c r="D230" s="3"/>
       <c r="E230" s="1"/>
       <c r="F230" s="1"/>
@@ -13616,7 +12747,6 @@
     </row>
     <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
-      <c r="C231" s="5"/>
       <c r="D231" s="3"/>
       <c r="E231" s="1"/>
       <c r="F231" s="1"/>
@@ -13635,7 +12765,6 @@
     </row>
     <row r="232" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
-      <c r="C232" s="5"/>
       <c r="D232" s="3"/>
       <c r="E232" s="1"/>
       <c r="F232" s="1"/>
@@ -13654,7 +12783,6 @@
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
-      <c r="C233" s="5"/>
       <c r="D233" s="3"/>
       <c r="E233" s="1"/>
       <c r="F233" s="1"/>
@@ -13673,7 +12801,6 @@
     </row>
     <row r="234" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
-      <c r="C234" s="5"/>
       <c r="D234" s="3"/>
       <c r="E234" s="1"/>
       <c r="F234" s="1"/>
@@ -13692,7 +12819,6 @@
     </row>
     <row r="235" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
-      <c r="C235" s="5"/>
       <c r="D235" s="3"/>
       <c r="E235" s="1"/>
       <c r="F235" s="1"/>
@@ -13711,7 +12837,6 @@
     </row>
     <row r="236" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
-      <c r="C236" s="5"/>
       <c r="D236" s="3"/>
       <c r="E236" s="1"/>
       <c r="F236" s="1"/>
@@ -13730,7 +12855,6 @@
     </row>
     <row r="237" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
-      <c r="C237" s="5"/>
       <c r="D237" s="3"/>
       <c r="E237" s="1"/>
       <c r="F237" s="1"/>
@@ -13749,7 +12873,6 @@
     </row>
     <row r="238" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
-      <c r="C238" s="5"/>
       <c r="D238" s="3"/>
       <c r="E238" s="1"/>
       <c r="F238" s="1"/>
@@ -13768,7 +12891,6 @@
     </row>
     <row r="239" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
-      <c r="C239" s="5"/>
       <c r="D239" s="3"/>
       <c r="E239" s="1"/>
       <c r="F239" s="1"/>
@@ -13787,7 +12909,6 @@
     </row>
     <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
-      <c r="C240" s="5"/>
       <c r="D240" s="3"/>
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
@@ -13806,7 +12927,6 @@
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
-      <c r="C241" s="5"/>
       <c r="D241" s="3"/>
       <c r="E241" s="1"/>
       <c r="F241" s="1"/>
@@ -13825,7 +12945,6 @@
     </row>
     <row r="242" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
-      <c r="C242" s="5"/>
       <c r="D242" s="3"/>
       <c r="E242" s="1"/>
       <c r="F242" s="1"/>
@@ -13844,7 +12963,6 @@
     </row>
     <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
-      <c r="C243" s="5"/>
       <c r="D243" s="3"/>
       <c r="E243" s="1"/>
       <c r="F243" s="1"/>
@@ -13863,7 +12981,6 @@
     </row>
     <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
-      <c r="C244" s="5"/>
       <c r="D244" s="3"/>
       <c r="E244" s="1"/>
       <c r="F244" s="1"/>
@@ -13882,7 +12999,6 @@
     </row>
     <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
-      <c r="C245" s="5"/>
       <c r="D245" s="3"/>
       <c r="E245" s="1"/>
       <c r="F245" s="1"/>
@@ -13901,7 +13017,6 @@
     </row>
     <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
-      <c r="C246" s="5"/>
       <c r="D246" s="3"/>
       <c r="E246" s="1"/>
       <c r="F246" s="1"/>
@@ -13920,7 +13035,6 @@
     </row>
     <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
-      <c r="C247" s="5"/>
       <c r="D247" s="3"/>
       <c r="E247" s="1"/>
       <c r="F247" s="1"/>
@@ -13939,7 +13053,6 @@
     </row>
     <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
-      <c r="C248" s="5"/>
       <c r="D248" s="3"/>
       <c r="E248" s="1"/>
       <c r="F248" s="1"/>
@@ -13958,7 +13071,6 @@
     </row>
     <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
-      <c r="C249" s="5"/>
       <c r="D249" s="3"/>
       <c r="E249" s="1"/>
       <c r="F249" s="1"/>
@@ -13977,7 +13089,6 @@
     </row>
     <row r="250" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
-      <c r="C250" s="5"/>
       <c r="D250" s="3"/>
       <c r="E250" s="1"/>
       <c r="F250" s="1"/>
@@ -13996,7 +13107,6 @@
     </row>
     <row r="251" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
-      <c r="C251" s="5"/>
       <c r="D251" s="3"/>
       <c r="E251" s="1"/>
       <c r="F251" s="1"/>
@@ -14015,7 +13125,6 @@
     </row>
     <row r="252" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
-      <c r="C252" s="5"/>
       <c r="D252" s="3"/>
       <c r="E252" s="1"/>
       <c r="F252" s="1"/>
@@ -14034,7 +13143,6 @@
     </row>
     <row r="253" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
-      <c r="C253" s="5"/>
       <c r="D253" s="3"/>
       <c r="E253" s="1"/>
       <c r="F253" s="1"/>
@@ -14053,7 +13161,6 @@
     </row>
     <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
-      <c r="C254" s="5"/>
       <c r="D254" s="3"/>
       <c r="E254" s="1"/>
       <c r="F254" s="1"/>
@@ -14072,7 +13179,6 @@
     </row>
     <row r="255" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
-      <c r="C255" s="5"/>
       <c r="D255" s="3"/>
       <c r="E255" s="1"/>
       <c r="F255" s="1"/>
@@ -14091,7 +13197,6 @@
     </row>
     <row r="256" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
-      <c r="C256" s="5"/>
       <c r="D256" s="3"/>
       <c r="E256" s="1"/>
       <c r="F256" s="1"/>
@@ -14110,7 +13215,6 @@
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
-      <c r="C257" s="5"/>
       <c r="D257" s="3"/>
       <c r="E257" s="1"/>
       <c r="F257" s="1"/>
@@ -14129,7 +13233,6 @@
     </row>
     <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
-      <c r="C258" s="5"/>
       <c r="D258" s="3"/>
       <c r="E258" s="1"/>
       <c r="F258" s="1"/>
@@ -14148,7 +13251,6 @@
     </row>
     <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
-      <c r="C259" s="5"/>
       <c r="D259" s="3"/>
       <c r="E259" s="1"/>
       <c r="F259" s="1"/>
@@ -14167,7 +13269,6 @@
     </row>
     <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
-      <c r="C260" s="5"/>
       <c r="D260" s="3"/>
       <c r="E260" s="1"/>
       <c r="F260" s="1"/>
@@ -14186,7 +13287,6 @@
     </row>
     <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
-      <c r="C261" s="5"/>
       <c r="D261" s="3"/>
       <c r="E261" s="1"/>
       <c r="F261" s="1"/>
@@ -14205,7 +13305,6 @@
     </row>
     <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
-      <c r="C262" s="5"/>
       <c r="D262" s="3"/>
       <c r="E262" s="1"/>
       <c r="F262" s="1"/>
@@ -14224,7 +13323,6 @@
     </row>
     <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
-      <c r="C263" s="5"/>
       <c r="D263" s="3"/>
       <c r="E263" s="1"/>
       <c r="F263" s="1"/>
@@ -14243,7 +13341,6 @@
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
-      <c r="C264" s="5"/>
       <c r="D264" s="3"/>
       <c r="E264" s="1"/>
       <c r="F264" s="1"/>
@@ -14262,7 +13359,6 @@
     </row>
     <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
-      <c r="C265" s="5"/>
       <c r="D265" s="3"/>
       <c r="E265" s="1"/>
       <c r="F265" s="1"/>
@@ -14281,7 +13377,6 @@
     </row>
     <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
-      <c r="C266" s="5"/>
       <c r="D266" s="3"/>
       <c r="E266" s="1"/>
       <c r="F266" s="1"/>
@@ -14300,7 +13395,6 @@
     </row>
     <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
-      <c r="C267" s="5"/>
       <c r="D267" s="3"/>
       <c r="E267" s="1"/>
       <c r="F267" s="1"/>
@@ -14319,7 +13413,6 @@
     </row>
     <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
-      <c r="C268" s="5"/>
       <c r="D268" s="3"/>
       <c r="E268" s="1"/>
       <c r="F268" s="1"/>
@@ -14338,7 +13431,6 @@
     </row>
     <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
-      <c r="C269" s="5"/>
       <c r="D269" s="3"/>
       <c r="E269" s="1"/>
       <c r="F269" s="1"/>
@@ -14357,7 +13449,6 @@
     </row>
     <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
-      <c r="C270" s="5"/>
       <c r="D270" s="3"/>
       <c r="E270" s="1"/>
       <c r="F270" s="1"/>
@@ -14376,7 +13467,6 @@
     </row>
     <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
-      <c r="C271" s="5"/>
       <c r="D271" s="3"/>
       <c r="E271" s="1"/>
       <c r="F271" s="1"/>
@@ -14395,7 +13485,6 @@
     </row>
     <row r="272" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
-      <c r="C272" s="5"/>
       <c r="D272" s="3"/>
       <c r="E272" s="1"/>
       <c r="F272" s="1"/>
@@ -14414,7 +13503,6 @@
     </row>
     <row r="273" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
-      <c r="C273" s="5"/>
       <c r="D273" s="3"/>
       <c r="E273" s="1"/>
       <c r="F273" s="1"/>
@@ -14433,7 +13521,6 @@
     </row>
     <row r="274" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
-      <c r="C274" s="5"/>
       <c r="D274" s="3"/>
       <c r="E274" s="1"/>
       <c r="F274" s="1"/>
@@ -14452,7 +13539,6 @@
     </row>
     <row r="275" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
-      <c r="C275" s="5"/>
       <c r="D275" s="3"/>
       <c r="E275" s="1"/>
       <c r="F275" s="1"/>
@@ -14472,7 +13558,7 @@
     <row r="276" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
-      <c r="C276" s="5"/>
+      <c r="C276" s="2"/>
       <c r="D276" s="3"/>
       <c r="E276" s="1"/>
       <c r="F276" s="1"/>
@@ -15690,7 +14776,7 @@
       <c r="R336" s="1"/>
     </row>
     <row r="337" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A337" s="4"/>
+      <c r="A337" s="2"/>
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="3"/>
@@ -15930,7 +15016,7 @@
       <c r="R348" s="1"/>
     </row>
     <row r="349" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C349" s="2"/>
+      <c r="A349" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>